<commit_message>
noseqsej psy plutot que nosejpsy
</commit_message>
<xml_diff>
--- a/formats/excel/Formats R3A 12.xlsx
+++ b/formats/excel/Formats R3A 12.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Github/formats_pmeasyr/formats/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="405" windowWidth="24675" windowHeight="11220"/>
+    <workbookView xWindow="1460" yWindow="460" windowWidth="27340" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -72,9 +85,6 @@
     <t xml:space="preserve">Identifiant de séjour </t>
   </si>
   <si>
-    <t>NOSEJPSY</t>
-  </si>
-  <si>
     <t xml:space="preserve">Age du patient en années à la date de réalisation de l'acte </t>
   </si>
   <si>
@@ -190,6 +200,9 @@
   </si>
   <si>
     <t>ZAD</t>
+  </si>
+  <si>
+    <t>NOSEQSEJ</t>
   </si>
 </sst>
 </file>
@@ -244,7 +257,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Bureau">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -282,14 +295,14 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Bureau">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -319,12 +332,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -354,7 +367,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Bureau">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -531,15 +544,15 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -579,7 +592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -599,7 +612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -619,7 +632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -639,7 +652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -659,7 +672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -673,15 +686,15 @@
         <v>45</v>
       </c>
       <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -693,15 +706,15 @@
         <v>48</v>
       </c>
       <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="F8" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -713,15 +726,15 @@
         <v>51</v>
       </c>
       <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -733,15 +746,15 @@
         <v>52</v>
       </c>
       <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>25</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>26</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -753,15 +766,15 @@
         <v>57</v>
       </c>
       <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>27</v>
-      </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>28</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -773,15 +786,15 @@
         <v>59</v>
       </c>
       <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>30</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -793,15 +806,15 @@
         <v>64</v>
       </c>
       <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>31</v>
-      </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>32</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -813,15 +826,15 @@
         <v>65</v>
       </c>
       <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>33</v>
-      </c>
-      <c r="F14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>34</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -833,15 +846,15 @@
         <v>73</v>
       </c>
       <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>35</v>
-      </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>36</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -853,15 +866,15 @@
         <v>75</v>
       </c>
       <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>37</v>
-      </c>
-      <c r="F16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>38</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -873,15 +886,15 @@
         <v>79</v>
       </c>
       <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>39</v>
-      </c>
-      <c r="F17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>40</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -893,15 +906,15 @@
         <v>80</v>
       </c>
       <c r="E18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>41</v>
-      </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>42</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -913,15 +926,15 @@
         <v>83</v>
       </c>
       <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>43</v>
-      </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>44</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -933,15 +946,15 @@
         <v>84</v>
       </c>
       <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>45</v>
-      </c>
-      <c r="F20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>46</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -953,15 +966,15 @@
         <v>85</v>
       </c>
       <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>47</v>
-      </c>
-      <c r="F21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>48</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -973,15 +986,15 @@
         <v>86</v>
       </c>
       <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>49</v>
-      </c>
-      <c r="F22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>50</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -993,15 +1006,15 @@
         <v>87</v>
       </c>
       <c r="E23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>51</v>
-      </c>
-      <c r="F23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>52</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -1013,15 +1026,15 @@
         <v>93</v>
       </c>
       <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>53</v>
-      </c>
-      <c r="F24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>54</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1033,15 +1046,15 @@
         <v>94</v>
       </c>
       <c r="E25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>55</v>
-      </c>
-      <c r="F25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>56</v>
       </c>
       <c r="B26">
         <v>6</v>
@@ -1053,7 +1066,7 @@
         <v>100</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -1070,7 +1083,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1082,7 +1095,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>